<commit_message>
Conciliación bancaria - mejoras en el documento Excel (resumen)
</commit_message>
<xml_diff>
--- a/excel/bancosConciliacionBancaria.xlsx
+++ b/excel/bancosConciliacionBancaria.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
-    <sheet name="Propios no encontrados" sheetId="1" r:id="rId1"/>
-    <sheet name="Del banco no encontrados" sheetId="2" r:id="rId2"/>
-    <sheet name="Resumen no encontrados" sheetId="3" r:id="rId3"/>
+    <sheet name="1) Propios no encontrados" sheetId="1" r:id="rId1"/>
+    <sheet name="2) Contables no encontrados" sheetId="4" r:id="rId2"/>
+    <sheet name="3) Del banco no encontrados" sheetId="2" r:id="rId3"/>
+    <sheet name="4) Resumen no encontrados" sheetId="3" r:id="rId4"/>
+    <sheet name="5) Lista propios" sheetId="5" r:id="rId5"/>
+    <sheet name="6) Lista contables" sheetId="6" r:id="rId6"/>
+    <sheet name="7) Lista banco" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
   <si>
     <t>{{nombreCiaContabSeleccionada}}</t>
   </si>
@@ -85,15 +89,97 @@
   </si>
   <si>
     <t>{{table:items.cantidad}}</t>
+  </si>
+  <si>
+    <t>Movimientos bancarios (propios) no encontrados</t>
+  </si>
+  <si>
+    <t>Movimientos contables (propios) no encontrados</t>
+  </si>
+  <si>
+    <t>Descripción comprobante</t>
+  </si>
+  <si>
+    <t>Descripción partida</t>
+  </si>
+  <si>
+    <t>{{table:items.descripcionComprobante}}</t>
+  </si>
+  <si>
+    <t>{{table:items.descripcionPartida}}</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>{{table:items.referencia}}</t>
+  </si>
+  <si>
+    <t>Movimientos contables propios no encontrados</t>
+  </si>
+  <si>
+    <t>{{table:itemsContab.tipo}}</t>
+  </si>
+  <si>
+    <t>{{table:itemsContab.cantidad}}</t>
+  </si>
+  <si>
+    <t>{{table:itemsContab.monto}}</t>
+  </si>
+  <si>
+    <t>{{table:itemsContab.tipoReg}}</t>
+  </si>
+  <si>
+    <t>bancos</t>
+  </si>
+  <si>
+    <t>contab</t>
+  </si>
+  <si>
+    <t>{{table:items.conciliadoBancos}}</t>
+  </si>
+  <si>
+    <t>{{table:items.conciliadoContab}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movimientos bancarios propios </t>
+  </si>
+  <si>
+    <t>Movimientos desde la contabilidad</t>
+  </si>
+  <si>
+    <t>{{table:items.comprobante}}</t>
+  </si>
+  <si>
+    <t>Movimientos bancarios del banco</t>
+  </si>
+  <si>
+    <t>{{table:items.conciliado}}</t>
+  </si>
+  <si>
+    <t>Conciliado en bancos y contab</t>
+  </si>
+  <si>
+    <t>{{table:items.consecutivoMovPropio}}</t>
+  </si>
+  <si>
+    <t>{{table:items.consecutivoMovContab}}</t>
+  </si>
+  <si>
+    <t>{{table:items.consecutivoMovBanco}}</t>
+  </si>
+  <si>
+    <t>Conciliado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00;\(#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="#"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -215,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,15 +346,79 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -277,7 +427,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -311,6 +511,71 @@
         <b/>
         <i/>
         <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
     <dxf>
@@ -624,50 +889,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="19" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
     <row r="3" spans="1:9" ht="18.75" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
       <c r="H3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" s="8" t="s">
@@ -692,7 +961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="26.25">
+    <row r="7" spans="1:9" ht="27.6">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>9</v>
@@ -732,7 +1001,7 @@
     <mergeCell ref="B4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:I10000">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>$I7 &lt;&gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -743,61 +1012,199 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:I7"/>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1">
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="28" customFormat="1" ht="27.6">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="H8" s="15"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B7:I10000">
+    <cfRule type="expression" dxfId="27" priority="2">
+      <formula>$I7 &lt;&gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="15.75">
+    <row r="1" spans="2:11">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.6">
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="11" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="19" t="s">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -816,34 +1223,46 @@
       <c r="G6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="2:9" ht="26.25">
-      <c r="B7" s="7" t="s">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" s="28" customFormat="1" ht="55.2">
+      <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="K7" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -853,102 +1272,596 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:I7">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$I7 &lt;&gt; 0</formula>
+  <conditionalFormatting sqref="B7:K7">
+    <cfRule type="expression" dxfId="26" priority="5">
+      <formula>$K7 &lt;&gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H10000">
+    <cfRule type="expression" dxfId="25" priority="4">
+      <formula>$H7="no"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="3">
+      <formula>$H7="si"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I10000">
+    <cfRule type="expression" dxfId="23" priority="2">
+      <formula>$I7="no"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="1">
+      <formula>$I7="si"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:H7"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15.75">
+    <row r="1" spans="2:8">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.6">
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
       <c r="H3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:8" ht="15.6">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.6">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.6">
+      <c r="B6" s="10"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="E7" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="E9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" s="28" customFormat="1" ht="27.6">
+      <c r="E10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="E15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="E17" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" s="28" customFormat="1" ht="27.6">
+      <c r="E18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E15:G15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10:H100000">
+    <cfRule type="expression" dxfId="21" priority="9">
+      <formula>$H10 &lt;&gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" customWidth="1"/>
+    <col min="7" max="7" width="41.77734375" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="15.6" customHeight="1">
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="26.25">
+    </row>
+    <row r="7" spans="2:10" ht="15.6" customHeight="1">
+      <c r="B7" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E3:G3"/>
+  <mergeCells count="4">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H7:H10000">
+    <cfRule type="expression" dxfId="15" priority="1">
+      <formula>$H7 = "no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="15.6">
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="69">
+      <c r="B7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H7:H10000">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$H7 = "no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="15.6">
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="96.6">
+      <c r="B7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:H7">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>$H7 &lt;&gt; 0</formula>
+  <conditionalFormatting sqref="H7:H10000">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$H7 = "no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J10000">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$J7 = "no"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>